<commit_message>
just in case you don't have it
</commit_message>
<xml_diff>
--- a/Molecular Structures Real/Descriptors 2.xlsx
+++ b/Molecular Structures Real/Descriptors 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14360" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14360" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10665,9 +10665,9 @@
   <dimension ref="A1:S75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5360" activePane="bottomLeft"/>
-      <selection activeCell="K1" sqref="K1:P1048576"/>
-      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
+      <pane ySplit="5360"/>
+      <selection activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>